<commit_message>
updated relay settings to match the device integration test - A
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Integration_Test_01/relay_settings/relay_parameters.xlsx
+++ b/DistributionSystems/SimulinkOpal/Integration_Test_01/relay_settings/relay_parameters.xlsx
@@ -68,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,26 +80,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -187,15 +167,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,7 +187,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>164523</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6225872" cy="4742452"/>
@@ -761,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +849,7 @@
         <v>0.5</v>
       </c>
       <c r="G2" s="7">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -946,7 +917,7 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="7">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -1063,787 +1034,39 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C5" s="8">
-        <v>5</v>
-      </c>
-      <c r="D5" s="8">
-        <v>12</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="7">
-        <v>50</v>
-      </c>
-      <c r="H5" s="10">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7">
-        <v>20</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L5" s="7">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P5" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>1</v>
-      </c>
-      <c r="R5" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S5" s="7">
-        <v>2</v>
-      </c>
-      <c r="T5" s="7">
-        <v>3</v>
-      </c>
-      <c r="U5" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V5" s="7">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C6" s="8">
-        <v>5</v>
-      </c>
-      <c r="D6" s="8">
-        <v>12</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="7">
-        <v>250</v>
-      </c>
-      <c r="H6" s="10">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7">
-        <v>20</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L6" s="7">
-        <v>1</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O6" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P6" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S6" s="7">
-        <v>2</v>
-      </c>
-      <c r="T6" s="7">
-        <v>3</v>
-      </c>
-      <c r="U6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V6" s="7">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C7" s="8">
-        <v>5</v>
-      </c>
-      <c r="D7" s="8">
-        <v>12</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="7">
-        <v>400</v>
-      </c>
-      <c r="H7" s="10">
-        <v>1</v>
-      </c>
-      <c r="I7" s="7">
-        <v>20</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L7" s="7">
-        <v>1</v>
-      </c>
-      <c r="M7" s="7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O7" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P7" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>1</v>
-      </c>
-      <c r="R7" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S7" s="7">
-        <v>2</v>
-      </c>
-      <c r="T7" s="7">
-        <v>3</v>
-      </c>
-      <c r="U7" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V7" s="7">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C8" s="8">
-        <v>5</v>
-      </c>
-      <c r="D8" s="8">
-        <v>12</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="7">
-        <v>50</v>
-      </c>
-      <c r="H8" s="10">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7">
-        <v>20</v>
-      </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L8" s="7">
-        <v>1</v>
-      </c>
-      <c r="M8" s="7">
-        <v>1</v>
-      </c>
-      <c r="N8" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O8" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P8" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>1</v>
-      </c>
-      <c r="R8" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S8" s="7">
-        <v>2</v>
-      </c>
-      <c r="T8" s="7">
-        <v>3</v>
-      </c>
-      <c r="U8" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V8" s="7">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C9" s="8">
-        <v>5</v>
-      </c>
-      <c r="D9" s="8">
-        <v>12</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="7">
-        <v>600</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7">
-        <v>20</v>
-      </c>
-      <c r="J9" s="7">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L9" s="7">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O9" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P9" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>1</v>
-      </c>
-      <c r="R9" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S9" s="7">
-        <v>2</v>
-      </c>
-      <c r="T9" s="7">
-        <v>3</v>
-      </c>
-      <c r="U9" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V9" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7">
-        <v>480</v>
-      </c>
-      <c r="C10" s="8">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8">
-        <v>12</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="7">
-        <v>600</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="7">
-        <v>20</v>
-      </c>
-      <c r="J10" s="7">
-        <v>0</v>
-      </c>
-      <c r="K10" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L10" s="7">
-        <v>1</v>
-      </c>
-      <c r="M10" s="7">
-        <v>1</v>
-      </c>
-      <c r="N10" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O10" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P10" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="7">
-        <v>1</v>
-      </c>
-      <c r="R10" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S10" s="7">
-        <v>2</v>
-      </c>
-      <c r="T10" s="7">
-        <v>3</v>
-      </c>
-      <c r="U10" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V10" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7">
-        <v>4160</v>
-      </c>
-      <c r="C11" s="8">
-        <v>5</v>
-      </c>
-      <c r="D11" s="8">
-        <v>12</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="7">
-        <v>600</v>
-      </c>
-      <c r="H11" s="10">
-        <v>1</v>
-      </c>
-      <c r="I11" s="7">
-        <v>20</v>
-      </c>
-      <c r="J11" s="7">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L11" s="7">
-        <v>1</v>
-      </c>
-      <c r="M11" s="7">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O11" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P11" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>1</v>
-      </c>
-      <c r="R11" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S11" s="7">
-        <v>2</v>
-      </c>
-      <c r="T11" s="7">
-        <v>3</v>
-      </c>
-      <c r="U11" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V11" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7">
-        <v>4160</v>
-      </c>
-      <c r="C12" s="8">
-        <v>5</v>
-      </c>
-      <c r="D12" s="8">
-        <v>12</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G12" s="7">
-        <v>600</v>
-      </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="7">
-        <v>20</v>
-      </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L12" s="7">
-        <v>1</v>
-      </c>
-      <c r="M12" s="7">
-        <v>1</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O12" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P12" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>1</v>
-      </c>
-      <c r="R12" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S12" s="7">
-        <v>2</v>
-      </c>
-      <c r="T12" s="7">
-        <v>3</v>
-      </c>
-      <c r="U12" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V12" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C13" s="8">
-        <v>5</v>
-      </c>
-      <c r="D13" s="8">
-        <v>12</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="7">
-        <v>250</v>
-      </c>
-      <c r="H13" s="10">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7">
-        <v>20</v>
-      </c>
-      <c r="J13" s="7">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L13" s="7">
-        <v>1</v>
-      </c>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O13" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P13" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>1</v>
-      </c>
-      <c r="R13" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S13" s="7">
-        <v>2</v>
-      </c>
-      <c r="T13" s="7">
-        <v>3</v>
-      </c>
-      <c r="U13" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V13" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7">
-        <v>480</v>
-      </c>
-      <c r="C14" s="8">
-        <v>5</v>
-      </c>
-      <c r="D14" s="8">
-        <v>12</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="7">
-        <v>600</v>
-      </c>
-      <c r="H14" s="11">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7">
-        <v>20</v>
-      </c>
-      <c r="J14" s="7">
-        <v>0</v>
-      </c>
-      <c r="K14" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L14" s="7">
-        <v>1</v>
-      </c>
-      <c r="M14" s="7">
-        <v>1</v>
-      </c>
-      <c r="N14" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O14" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P14" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>1</v>
-      </c>
-      <c r="R14" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S14" s="7">
-        <v>2</v>
-      </c>
-      <c r="T14" s="7">
-        <v>3</v>
-      </c>
-      <c r="U14" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V14" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7">
-        <v>480</v>
-      </c>
-      <c r="C15" s="8">
-        <v>5</v>
-      </c>
-      <c r="D15" s="8">
-        <v>12</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G15" s="7">
-        <v>2500</v>
-      </c>
-      <c r="H15" s="12">
-        <v>1</v>
-      </c>
-      <c r="I15" s="7">
-        <v>20</v>
-      </c>
-      <c r="J15" s="7">
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L15" s="7">
-        <v>1</v>
-      </c>
-      <c r="M15" s="7">
-        <v>1</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O15" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P15" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>1</v>
-      </c>
-      <c r="R15" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S15" s="7">
-        <v>2</v>
-      </c>
-      <c r="T15" s="7">
-        <v>3</v>
-      </c>
-      <c r="U15" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V15" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="A9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
executed the case - modified parameters
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Integration_Test_01/relay_settings/relay_parameters.xlsx
+++ b/DistributionSystems/SimulinkOpal/Integration_Test_01/relay_settings/relay_parameters.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>0.5</v>
       </c>
       <c r="G2" s="7">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -917,7 +917,7 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="7">
-        <v>250</v>
+        <v>600</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -966,72 +966,12 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>13800</v>
-      </c>
-      <c r="C4" s="8">
-        <v>5</v>
-      </c>
-      <c r="D4" s="8">
-        <v>12</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="7">
-        <v>600</v>
-      </c>
-      <c r="H4" s="10">
-        <v>1</v>
-      </c>
-      <c r="I4" s="7">
-        <v>20</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0</v>
-      </c>
-      <c r="K4" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L4" s="7">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7">
-        <v>1</v>
-      </c>
-      <c r="N4" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="O4" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P4" s="7">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>1</v>
-      </c>
-      <c r="R4" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="S4" s="7">
-        <v>2</v>
-      </c>
-      <c r="T4" s="7">
-        <v>3</v>
-      </c>
-      <c r="U4" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="V4" s="7">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>

</xml_diff>